<commit_message>
- Add some image distortions
</commit_message>
<xml_diff>
--- a/CNN_Calc.xlsx
+++ b/CNN_Calc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Layer Type</t>
   </si>
@@ -469,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O16"/>
+  <dimension ref="B1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +757,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="1">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -783,7 +783,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="1">
-        <v>43</v>
+        <v>300</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -805,12 +805,27 @@
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1">
+        <v>200</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -859,6 +874,17 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="F1:H1"/>

</xml_diff>